<commit_message>
Fixing TC01, TC05, TC06
</commit_message>
<xml_diff>
--- a/Excel/Excel_Config.xlsx
+++ b/Excel/Excel_Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\ICONS\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC49144-1803-4AC6-BE33-595DA9B43652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A71782FF-B43D-4D0D-A45A-2321F34CE6D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="3" xr2:uid="{6FC7654C-3A1B-4451-AA94-4524C316DE43}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="API_DB" sheetId="2" r:id="rId3"/>
     <sheet name="ICONS" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -400,7 +400,7 @@
     <t>LOG_FNSONLAD_PASSWORD</t>
   </si>
   <si>
-    <t>17060</t>
+    <t>99971</t>
   </si>
 </sst>
 </file>

</xml_diff>